<commit_message>
Initial commit: DSHI Field Pad dashboard project
</commit_message>
<xml_diff>
--- a/assembly_data.xlsx
+++ b/assembly_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSHI_RPA\APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B0EE91-00E7-4313-AFC9-61A0964F7982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0F88C7-0338-4251-84DF-3E117A176E15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" activeTab="2" xr2:uid="{A67438B1-42EE-4A32-B49D-16C67929AFA2}"/>
   </bookViews>
@@ -15347,7 +15347,7 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15356,7 +15356,7 @@
       </c>
       <c r="B3" s="14">
         <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(1, 100)</f>
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15365,7 +15365,7 @@
       </c>
       <c r="B4" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15374,7 +15374,7 @@
       </c>
       <c r="B5" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15383,7 +15383,7 @@
       </c>
       <c r="B6" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15392,7 +15392,7 @@
       </c>
       <c r="B7" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15401,7 +15401,7 @@
       </c>
       <c r="B8" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15410,7 +15410,7 @@
       </c>
       <c r="B9" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15419,7 +15419,7 @@
       </c>
       <c r="B10" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15428,7 +15428,7 @@
       </c>
       <c r="B11" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15437,7 +15437,7 @@
       </c>
       <c r="B12" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15455,7 +15455,7 @@
       </c>
       <c r="B14" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15464,7 +15464,7 @@
       </c>
       <c r="B15" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15473,7 +15473,7 @@
       </c>
       <c r="B16" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15482,7 +15482,7 @@
       </c>
       <c r="B17" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15491,7 +15491,7 @@
       </c>
       <c r="B18" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15500,7 +15500,7 @@
       </c>
       <c r="B19" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15509,7 +15509,7 @@
       </c>
       <c r="B20" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15518,7 +15518,7 @@
       </c>
       <c r="B21" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15527,7 +15527,7 @@
       </c>
       <c r="B22" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15536,7 +15536,7 @@
       </c>
       <c r="B23" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15545,7 +15545,7 @@
       </c>
       <c r="B24" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15554,7 +15554,7 @@
       </c>
       <c r="B25" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15563,7 +15563,7 @@
       </c>
       <c r="B26" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15572,7 +15572,7 @@
       </c>
       <c r="B27" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15581,7 +15581,7 @@
       </c>
       <c r="B28" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="B29" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15599,7 +15599,7 @@
       </c>
       <c r="B30" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15608,7 +15608,7 @@
       </c>
       <c r="B31" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15617,7 +15617,7 @@
       </c>
       <c r="B32" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15626,7 +15626,7 @@
       </c>
       <c r="B33" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15635,7 +15635,7 @@
       </c>
       <c r="B34" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15644,7 +15644,7 @@
       </c>
       <c r="B35" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15653,7 +15653,7 @@
       </c>
       <c r="B36" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15662,7 +15662,7 @@
       </c>
       <c r="B37" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15671,7 +15671,7 @@
       </c>
       <c r="B38" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15680,7 +15680,7 @@
       </c>
       <c r="B39" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15689,7 +15689,7 @@
       </c>
       <c r="B40" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="B41" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15707,7 +15707,7 @@
       </c>
       <c r="B42" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15716,7 +15716,7 @@
       </c>
       <c r="B43" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15725,7 +15725,7 @@
       </c>
       <c r="B44" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15734,7 +15734,7 @@
       </c>
       <c r="B45" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15743,7 +15743,7 @@
       </c>
       <c r="B46" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15752,7 +15752,7 @@
       </c>
       <c r="B47" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15761,7 +15761,7 @@
       </c>
       <c r="B48" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15770,7 +15770,7 @@
       </c>
       <c r="B49" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15779,7 +15779,7 @@
       </c>
       <c r="B50" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15788,7 +15788,7 @@
       </c>
       <c r="B51" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15797,7 +15797,7 @@
       </c>
       <c r="B52" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15806,7 +15806,7 @@
       </c>
       <c r="B53" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15815,7 +15815,7 @@
       </c>
       <c r="B54" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15824,7 +15824,7 @@
       </c>
       <c r="B55" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15833,7 +15833,7 @@
       </c>
       <c r="B56" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15842,7 +15842,7 @@
       </c>
       <c r="B57" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15851,7 +15851,7 @@
       </c>
       <c r="B58" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15860,7 +15860,7 @@
       </c>
       <c r="B59" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15869,7 +15869,7 @@
       </c>
       <c r="B60" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15878,7 +15878,7 @@
       </c>
       <c r="B61" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15887,7 +15887,7 @@
       </c>
       <c r="B62" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15896,7 +15896,7 @@
       </c>
       <c r="B63" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="B64" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15914,7 +15914,7 @@
       </c>
       <c r="B65" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15923,7 +15923,7 @@
       </c>
       <c r="B66" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15932,7 +15932,7 @@
       </c>
       <c r="B67" s="14">
         <f t="shared" ref="B67:B130" ca="1" si="1">RANDBETWEEN(1, 100)</f>
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15941,7 +15941,7 @@
       </c>
       <c r="B68" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15950,7 +15950,7 @@
       </c>
       <c r="B69" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15959,7 +15959,7 @@
       </c>
       <c r="B70" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15968,7 +15968,7 @@
       </c>
       <c r="B71" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15977,7 +15977,7 @@
       </c>
       <c r="B72" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15986,7 +15986,7 @@
       </c>
       <c r="B73" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15995,7 +15995,7 @@
       </c>
       <c r="B74" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16004,7 +16004,7 @@
       </c>
       <c r="B75" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16013,7 +16013,7 @@
       </c>
       <c r="B76" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16022,7 +16022,7 @@
       </c>
       <c r="B77" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16031,7 +16031,7 @@
       </c>
       <c r="B78" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16040,7 +16040,7 @@
       </c>
       <c r="B79" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16049,7 +16049,7 @@
       </c>
       <c r="B80" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16058,7 +16058,7 @@
       </c>
       <c r="B81" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16067,7 +16067,7 @@
       </c>
       <c r="B82" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16076,7 +16076,7 @@
       </c>
       <c r="B83" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16085,7 +16085,7 @@
       </c>
       <c r="B84" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16094,7 +16094,7 @@
       </c>
       <c r="B85" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16103,7 +16103,7 @@
       </c>
       <c r="B86" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16112,7 +16112,7 @@
       </c>
       <c r="B87" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16121,7 +16121,7 @@
       </c>
       <c r="B88" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16130,7 +16130,7 @@
       </c>
       <c r="B89" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16139,7 +16139,7 @@
       </c>
       <c r="B90" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16148,7 +16148,7 @@
       </c>
       <c r="B91" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16157,7 +16157,7 @@
       </c>
       <c r="B92" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="B93" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16175,7 +16175,7 @@
       </c>
       <c r="B94" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16184,7 +16184,7 @@
       </c>
       <c r="B95" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16193,7 +16193,7 @@
       </c>
       <c r="B96" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16202,7 +16202,7 @@
       </c>
       <c r="B97" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16211,7 +16211,7 @@
       </c>
       <c r="B98" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16220,7 +16220,7 @@
       </c>
       <c r="B99" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16229,7 +16229,7 @@
       </c>
       <c r="B100" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16238,7 +16238,7 @@
       </c>
       <c r="B101" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16247,7 +16247,7 @@
       </c>
       <c r="B102" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16256,7 +16256,7 @@
       </c>
       <c r="B103" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16265,7 +16265,7 @@
       </c>
       <c r="B104" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16274,7 +16274,7 @@
       </c>
       <c r="B105" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16283,7 +16283,7 @@
       </c>
       <c r="B106" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16292,7 +16292,7 @@
       </c>
       <c r="B107" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16301,7 +16301,7 @@
       </c>
       <c r="B108" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16310,7 +16310,7 @@
       </c>
       <c r="B109" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16319,7 +16319,7 @@
       </c>
       <c r="B110" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16328,7 +16328,7 @@
       </c>
       <c r="B111" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16337,7 +16337,7 @@
       </c>
       <c r="B112" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16346,7 +16346,7 @@
       </c>
       <c r="B113" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16355,7 +16355,7 @@
       </c>
       <c r="B114" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16364,7 +16364,7 @@
       </c>
       <c r="B115" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16373,7 +16373,7 @@
       </c>
       <c r="B116" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16382,7 +16382,7 @@
       </c>
       <c r="B117" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16391,7 +16391,7 @@
       </c>
       <c r="B118" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="119" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16400,7 +16400,7 @@
       </c>
       <c r="B119" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="120" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16409,7 +16409,7 @@
       </c>
       <c r="B120" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16418,7 +16418,7 @@
       </c>
       <c r="B121" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16427,7 +16427,7 @@
       </c>
       <c r="B122" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>98</v>
       </c>
     </row>
     <row r="123" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16436,7 +16436,7 @@
       </c>
       <c r="B123" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16445,7 +16445,7 @@
       </c>
       <c r="B124" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="125" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16454,7 +16454,7 @@
       </c>
       <c r="B125" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16463,7 +16463,7 @@
       </c>
       <c r="B126" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="127" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16472,7 +16472,7 @@
       </c>
       <c r="B127" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16481,7 +16481,7 @@
       </c>
       <c r="B128" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="129" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16490,7 +16490,7 @@
       </c>
       <c r="B129" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="130" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16499,7 +16499,7 @@
       </c>
       <c r="B130" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16508,7 +16508,7 @@
       </c>
       <c r="B131" s="14">
         <f t="shared" ref="B131:B194" ca="1" si="2">RANDBETWEEN(1, 100)</f>
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16517,7 +16517,7 @@
       </c>
       <c r="B132" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16526,7 +16526,7 @@
       </c>
       <c r="B133" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16535,7 +16535,7 @@
       </c>
       <c r="B134" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="135" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16544,7 +16544,7 @@
       </c>
       <c r="B135" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16553,7 +16553,7 @@
       </c>
       <c r="B136" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>84</v>
       </c>
     </row>
     <row r="137" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16562,7 +16562,7 @@
       </c>
       <c r="B137" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16571,7 +16571,7 @@
       </c>
       <c r="B138" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="139" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16580,7 +16580,7 @@
       </c>
       <c r="B139" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16589,7 +16589,7 @@
       </c>
       <c r="B140" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="141" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16598,7 +16598,7 @@
       </c>
       <c r="B141" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16607,7 +16607,7 @@
       </c>
       <c r="B142" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="143" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16616,7 +16616,7 @@
       </c>
       <c r="B143" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="144" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16625,7 +16625,7 @@
       </c>
       <c r="B144" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="145" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="B145" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="146" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16643,7 +16643,7 @@
       </c>
       <c r="B146" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16652,7 +16652,7 @@
       </c>
       <c r="B147" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="148" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16661,7 +16661,7 @@
       </c>
       <c r="B148" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="149" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16670,7 +16670,7 @@
       </c>
       <c r="B149" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16679,7 +16679,7 @@
       </c>
       <c r="B150" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="151" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16688,7 +16688,7 @@
       </c>
       <c r="B151" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16697,7 +16697,7 @@
       </c>
       <c r="B152" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16715,7 +16715,7 @@
       </c>
       <c r="B154" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="155" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16724,7 +16724,7 @@
       </c>
       <c r="B155" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="156" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16733,7 +16733,7 @@
       </c>
       <c r="B156" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="157" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16742,7 +16742,7 @@
       </c>
       <c r="B157" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="158" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16751,7 +16751,7 @@
       </c>
       <c r="B158" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16760,7 +16760,7 @@
       </c>
       <c r="B159" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="160" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16769,7 +16769,7 @@
       </c>
       <c r="B160" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="161" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16778,7 +16778,7 @@
       </c>
       <c r="B161" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="162" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16787,7 +16787,7 @@
       </c>
       <c r="B162" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="163" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16796,7 +16796,7 @@
       </c>
       <c r="B163" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="164" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16805,7 +16805,7 @@
       </c>
       <c r="B164" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>90</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16814,7 +16814,7 @@
       </c>
       <c r="B165" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="166" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16823,7 +16823,7 @@
       </c>
       <c r="B166" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16832,7 +16832,7 @@
       </c>
       <c r="B167" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="168" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16841,7 +16841,7 @@
       </c>
       <c r="B168" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="169" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16850,7 +16850,7 @@
       </c>
       <c r="B169" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16859,7 +16859,7 @@
       </c>
       <c r="B170" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="171" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16868,7 +16868,7 @@
       </c>
       <c r="B171" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16877,7 +16877,7 @@
       </c>
       <c r="B172" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>62</v>
       </c>
     </row>
     <row r="173" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16886,7 +16886,7 @@
       </c>
       <c r="B173" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="174" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16895,7 +16895,7 @@
       </c>
       <c r="B174" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="175" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16904,7 +16904,7 @@
       </c>
       <c r="B175" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16913,7 +16913,7 @@
       </c>
       <c r="B176" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>58</v>
       </c>
     </row>
     <row r="177" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16922,7 +16922,7 @@
       </c>
       <c r="B177" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="178" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16931,7 +16931,7 @@
       </c>
       <c r="B178" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="179" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16940,7 +16940,7 @@
       </c>
       <c r="B179" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="180" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16949,7 +16949,7 @@
       </c>
       <c r="B180" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="181" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16958,7 +16958,7 @@
       </c>
       <c r="B181" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16967,7 +16967,7 @@
       </c>
       <c r="B182" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>77</v>
       </c>
     </row>
     <row r="183" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16976,7 +16976,7 @@
       </c>
       <c r="B183" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="184" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16985,7 +16985,7 @@
       </c>
       <c r="B184" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="185" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -16994,7 +16994,7 @@
       </c>
       <c r="B185" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="186" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17003,7 +17003,7 @@
       </c>
       <c r="B186" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="187" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17012,7 +17012,7 @@
       </c>
       <c r="B187" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="188" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17021,7 +17021,7 @@
       </c>
       <c r="B188" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>69</v>
+        <v>93</v>
       </c>
     </row>
     <row r="189" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17030,7 +17030,7 @@
       </c>
       <c r="B189" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="190" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17039,7 +17039,7 @@
       </c>
       <c r="B190" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>96</v>
       </c>
     </row>
     <row r="191" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17048,7 +17048,7 @@
       </c>
       <c r="B191" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="192" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17057,7 +17057,7 @@
       </c>
       <c r="B192" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="193" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17066,7 +17066,7 @@
       </c>
       <c r="B193" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>63</v>
+        <v>96</v>
       </c>
     </row>
     <row r="194" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17075,7 +17075,7 @@
       </c>
       <c r="B194" s="14">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="195" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17084,7 +17084,7 @@
       </c>
       <c r="B195" s="14">
         <f t="shared" ref="B195:B258" ca="1" si="3">RANDBETWEEN(1, 100)</f>
-        <v>100</v>
+        <v>16</v>
       </c>
     </row>
     <row r="196" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17093,7 +17093,7 @@
       </c>
       <c r="B196" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>71</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17102,7 +17102,7 @@
       </c>
       <c r="B197" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="198" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17111,7 +17111,7 @@
       </c>
       <c r="B198" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="199" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17120,7 +17120,7 @@
       </c>
       <c r="B199" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="200" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17129,7 +17129,7 @@
       </c>
       <c r="B200" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>39</v>
       </c>
     </row>
     <row r="201" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17138,7 +17138,7 @@
       </c>
       <c r="B201" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17147,7 +17147,7 @@
       </c>
       <c r="B202" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>40</v>
       </c>
     </row>
     <row r="203" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17156,7 +17156,7 @@
       </c>
       <c r="B203" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17165,7 +17165,7 @@
       </c>
       <c r="B204" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17174,7 +17174,7 @@
       </c>
       <c r="B205" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="206" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17183,7 +17183,7 @@
       </c>
       <c r="B206" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="207" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17192,7 +17192,7 @@
       </c>
       <c r="B207" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="208" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17201,7 +17201,7 @@
       </c>
       <c r="B208" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="209" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17210,7 +17210,7 @@
       </c>
       <c r="B209" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="210" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17219,7 +17219,7 @@
       </c>
       <c r="B210" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="211" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17228,7 +17228,7 @@
       </c>
       <c r="B211" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17237,7 +17237,7 @@
       </c>
       <c r="B212" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="213" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17246,7 +17246,7 @@
       </c>
       <c r="B213" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>79</v>
       </c>
     </row>
     <row r="214" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17255,7 +17255,7 @@
       </c>
       <c r="B214" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>37</v>
       </c>
     </row>
     <row r="215" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17264,7 +17264,7 @@
       </c>
       <c r="B215" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="216" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17273,7 +17273,7 @@
       </c>
       <c r="B216" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17282,7 +17282,7 @@
       </c>
       <c r="B217" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="218" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17291,7 +17291,7 @@
       </c>
       <c r="B218" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="219" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17300,7 +17300,7 @@
       </c>
       <c r="B219" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="220" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17309,7 +17309,7 @@
       </c>
       <c r="B220" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="221" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17318,7 +17318,7 @@
       </c>
       <c r="B221" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17327,7 +17327,7 @@
       </c>
       <c r="B222" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="223" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17345,7 +17345,7 @@
       </c>
       <c r="B224" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="225" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17354,7 +17354,7 @@
       </c>
       <c r="B225" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>73</v>
       </c>
     </row>
     <row r="226" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17363,7 +17363,7 @@
       </c>
       <c r="B226" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>38</v>
       </c>
     </row>
     <row r="227" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17372,7 +17372,7 @@
       </c>
       <c r="B227" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="228" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17381,7 +17381,7 @@
       </c>
       <c r="B228" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="229" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17390,7 +17390,7 @@
       </c>
       <c r="B229" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>92</v>
       </c>
     </row>
     <row r="230" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17399,7 +17399,7 @@
       </c>
       <c r="B230" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="231" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17408,7 +17408,7 @@
       </c>
       <c r="B231" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="232" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17417,7 +17417,7 @@
       </c>
       <c r="B232" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="233" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17426,7 +17426,7 @@
       </c>
       <c r="B233" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>31</v>
       </c>
     </row>
     <row r="234" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17435,7 +17435,7 @@
       </c>
       <c r="B234" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>27</v>
       </c>
     </row>
     <row r="235" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17444,7 +17444,7 @@
       </c>
       <c r="B235" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="236" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17453,7 +17453,7 @@
       </c>
       <c r="B236" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>83</v>
+        <v>46</v>
       </c>
     </row>
     <row r="237" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17462,7 +17462,7 @@
       </c>
       <c r="B237" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="238" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17471,7 +17471,7 @@
       </c>
       <c r="B238" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>86</v>
       </c>
     </row>
     <row r="239" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17480,7 +17480,7 @@
       </c>
       <c r="B239" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>40</v>
       </c>
     </row>
     <row r="240" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17489,7 +17489,7 @@
       </c>
       <c r="B240" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="241" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17498,7 +17498,7 @@
       </c>
       <c r="B241" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="242" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17507,7 +17507,7 @@
       </c>
       <c r="B242" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="243" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17516,7 +17516,7 @@
       </c>
       <c r="B243" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="244" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17525,7 +17525,7 @@
       </c>
       <c r="B244" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>5</v>
       </c>
     </row>
     <row r="245" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17534,7 +17534,7 @@
       </c>
       <c r="B245" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="246" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17543,7 +17543,7 @@
       </c>
       <c r="B246" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="247" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="B247" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>80</v>
       </c>
     </row>
     <row r="248" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17561,7 +17561,7 @@
       </c>
       <c r="B248" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="249" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17570,7 +17570,7 @@
       </c>
       <c r="B249" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="250" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17579,7 +17579,7 @@
       </c>
       <c r="B250" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="251" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17588,7 +17588,7 @@
       </c>
       <c r="B251" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="252" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17597,7 +17597,7 @@
       </c>
       <c r="B252" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="253" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17606,7 +17606,7 @@
       </c>
       <c r="B253" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="254" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17615,7 +17615,7 @@
       </c>
       <c r="B254" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>72</v>
+        <v>9</v>
       </c>
     </row>
     <row r="255" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17624,7 +17624,7 @@
       </c>
       <c r="B255" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="256" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17633,7 +17633,7 @@
       </c>
       <c r="B256" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="257" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17642,7 +17642,7 @@
       </c>
       <c r="B257" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>86</v>
+        <v>18</v>
       </c>
     </row>
     <row r="258" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17651,7 +17651,7 @@
       </c>
       <c r="B258" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="259" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17660,7 +17660,7 @@
       </c>
       <c r="B259" s="14">
         <f t="shared" ref="B259:B322" ca="1" si="4">RANDBETWEEN(1, 100)</f>
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="260" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17669,7 +17669,7 @@
       </c>
       <c r="B260" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>84</v>
       </c>
     </row>
     <row r="261" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17678,7 +17678,7 @@
       </c>
       <c r="B261" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="262" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17687,7 +17687,7 @@
       </c>
       <c r="B262" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="263" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17696,7 +17696,7 @@
       </c>
       <c r="B263" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="264" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17705,7 +17705,7 @@
       </c>
       <c r="B264" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="265" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="B265" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="266" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17723,7 +17723,7 @@
       </c>
       <c r="B266" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="267" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17732,7 +17732,7 @@
       </c>
       <c r="B267" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="268" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17741,7 +17741,7 @@
       </c>
       <c r="B268" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="269" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17750,7 +17750,7 @@
       </c>
       <c r="B269" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="270" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17759,7 +17759,7 @@
       </c>
       <c r="B270" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="271" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17768,7 +17768,7 @@
       </c>
       <c r="B271" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="272" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17777,7 +17777,7 @@
       </c>
       <c r="B272" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="273" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17786,7 +17786,7 @@
       </c>
       <c r="B273" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="274" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17795,7 +17795,7 @@
       </c>
       <c r="B274" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="275" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17804,7 +17804,7 @@
       </c>
       <c r="B275" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
     <row r="276" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17813,7 +17813,7 @@
       </c>
       <c r="B276" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="277" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="B277" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="278" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17831,7 +17831,7 @@
       </c>
       <c r="B278" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="279" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17840,7 +17840,7 @@
       </c>
       <c r="B279" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="280" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17849,7 +17849,7 @@
       </c>
       <c r="B280" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="281" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17858,7 +17858,7 @@
       </c>
       <c r="B281" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="282" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17867,7 +17867,7 @@
       </c>
       <c r="B282" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="283" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17876,7 +17876,7 @@
       </c>
       <c r="B283" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="284" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17885,7 +17885,7 @@
       </c>
       <c r="B284" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="285" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17894,7 +17894,7 @@
       </c>
       <c r="B285" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="286" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17903,7 +17903,7 @@
       </c>
       <c r="B286" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="287" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17912,7 +17912,7 @@
       </c>
       <c r="B287" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="288" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17921,7 +17921,7 @@
       </c>
       <c r="B288" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="289" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17930,7 +17930,7 @@
       </c>
       <c r="B289" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17939,7 +17939,7 @@
       </c>
       <c r="B290" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="291" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17948,7 +17948,7 @@
       </c>
       <c r="B291" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="292" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17957,7 +17957,7 @@
       </c>
       <c r="B292" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="293" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17966,7 +17966,7 @@
       </c>
       <c r="B293" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>23</v>
+        <v>85</v>
       </c>
     </row>
     <row r="294" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17975,7 +17975,7 @@
       </c>
       <c r="B294" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>92</v>
       </c>
     </row>
     <row r="295" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17984,7 +17984,7 @@
       </c>
       <c r="B295" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="296" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -17993,7 +17993,7 @@
       </c>
       <c r="B296" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="297" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18002,7 +18002,7 @@
       </c>
       <c r="B297" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="298" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18011,7 +18011,7 @@
       </c>
       <c r="B298" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="299" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18020,7 +18020,7 @@
       </c>
       <c r="B299" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="300" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18029,7 +18029,7 @@
       </c>
       <c r="B300" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="301" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18038,7 +18038,7 @@
       </c>
       <c r="B301" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="302" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18047,7 +18047,7 @@
       </c>
       <c r="B302" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>76</v>
+        <v>11</v>
       </c>
     </row>
     <row r="303" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18056,7 +18056,7 @@
       </c>
       <c r="B303" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18065,7 +18065,7 @@
       </c>
       <c r="B304" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="305" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="B305" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>24</v>
+        <v>91</v>
       </c>
     </row>
     <row r="306" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18083,7 +18083,7 @@
       </c>
       <c r="B306" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>6</v>
       </c>
     </row>
     <row r="307" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18092,7 +18092,7 @@
       </c>
       <c r="B307" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="308" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18101,7 +18101,7 @@
       </c>
       <c r="B308" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="309" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18110,7 +18110,7 @@
       </c>
       <c r="B309" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="310" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18119,7 +18119,7 @@
       </c>
       <c r="B310" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="311" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18128,7 +18128,7 @@
       </c>
       <c r="B311" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="312" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18137,7 +18137,7 @@
       </c>
       <c r="B312" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="313" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18146,7 +18146,7 @@
       </c>
       <c r="B313" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="314" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18155,7 +18155,7 @@
       </c>
       <c r="B314" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="315" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18164,7 +18164,7 @@
       </c>
       <c r="B315" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="316" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18173,7 +18173,7 @@
       </c>
       <c r="B316" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="317" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18182,7 +18182,7 @@
       </c>
       <c r="B317" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="318" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18191,7 +18191,7 @@
       </c>
       <c r="B318" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="319" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18200,7 +18200,7 @@
       </c>
       <c r="B319" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="320" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18209,7 +18209,7 @@
       </c>
       <c r="B320" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>99</v>
       </c>
     </row>
     <row r="321" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18218,7 +18218,7 @@
       </c>
       <c r="B321" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18227,7 +18227,7 @@
       </c>
       <c r="B322" s="14">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="323" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18236,7 +18236,7 @@
       </c>
       <c r="B323" s="14">
         <f t="shared" ref="B323:B374" ca="1" si="5">RANDBETWEEN(1, 100)</f>
-        <v>97</v>
+        <v>11</v>
       </c>
     </row>
     <row r="324" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18245,7 +18245,7 @@
       </c>
       <c r="B324" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="325" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18254,7 +18254,7 @@
       </c>
       <c r="B325" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="326" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18263,7 +18263,7 @@
       </c>
       <c r="B326" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="327" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18272,7 +18272,7 @@
       </c>
       <c r="B327" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="328" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18281,7 +18281,7 @@
       </c>
       <c r="B328" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="329" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18299,7 +18299,7 @@
       </c>
       <c r="B330" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="331" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18308,7 +18308,7 @@
       </c>
       <c r="B331" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="332" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18317,7 +18317,7 @@
       </c>
       <c r="B332" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="333" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18326,7 +18326,7 @@
       </c>
       <c r="B333" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>89</v>
       </c>
     </row>
     <row r="334" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18335,7 +18335,7 @@
       </c>
       <c r="B334" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="335" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18344,7 +18344,7 @@
       </c>
       <c r="B335" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>97</v>
+        <v>4</v>
       </c>
     </row>
     <row r="336" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18353,7 +18353,7 @@
       </c>
       <c r="B336" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="337" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18362,7 +18362,7 @@
       </c>
       <c r="B337" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="338" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18371,7 +18371,7 @@
       </c>
       <c r="B338" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="339" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18380,7 +18380,7 @@
       </c>
       <c r="B339" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="340" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18389,7 +18389,7 @@
       </c>
       <c r="B340" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="341" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18398,7 +18398,7 @@
       </c>
       <c r="B341" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="342" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18407,7 +18407,7 @@
       </c>
       <c r="B342" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="343" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18416,7 +18416,7 @@
       </c>
       <c r="B343" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="344" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18425,7 +18425,7 @@
       </c>
       <c r="B344" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>98</v>
+        <v>46</v>
       </c>
     </row>
     <row r="345" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18434,7 +18434,7 @@
       </c>
       <c r="B345" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="346" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18443,7 +18443,7 @@
       </c>
       <c r="B346" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>98</v>
+        <v>39</v>
       </c>
     </row>
     <row r="347" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18452,7 +18452,7 @@
       </c>
       <c r="B347" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="348" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18461,7 +18461,7 @@
       </c>
       <c r="B348" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>39</v>
+        <v>85</v>
       </c>
     </row>
     <row r="349" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18470,7 +18470,7 @@
       </c>
       <c r="B349" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="350" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18479,7 +18479,7 @@
       </c>
       <c r="B350" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>54</v>
+        <v>12</v>
       </c>
     </row>
     <row r="351" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18488,7 +18488,7 @@
       </c>
       <c r="B351" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="352" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18497,7 +18497,7 @@
       </c>
       <c r="B352" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="353" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18506,7 +18506,7 @@
       </c>
       <c r="B353" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>69</v>
+        <v>10</v>
       </c>
     </row>
     <row r="354" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18515,7 +18515,7 @@
       </c>
       <c r="B354" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="355" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18524,7 +18524,7 @@
       </c>
       <c r="B355" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="356" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18533,7 +18533,7 @@
       </c>
       <c r="B356" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="357" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18551,7 +18551,7 @@
       </c>
       <c r="B358" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="359" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18560,7 +18560,7 @@
       </c>
       <c r="B359" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>87</v>
+        <v>25</v>
       </c>
     </row>
     <row r="360" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18569,7 +18569,7 @@
       </c>
       <c r="B360" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="361" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18578,7 +18578,7 @@
       </c>
       <c r="B361" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>33</v>
+        <v>93</v>
       </c>
     </row>
     <row r="362" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18587,7 +18587,7 @@
       </c>
       <c r="B362" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="363" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18596,7 +18596,7 @@
       </c>
       <c r="B363" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="364" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18605,7 +18605,7 @@
       </c>
       <c r="B364" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="365" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18614,7 +18614,7 @@
       </c>
       <c r="B365" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="366" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18623,7 +18623,7 @@
       </c>
       <c r="B366" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="367" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18632,7 +18632,7 @@
       </c>
       <c r="B367" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="368" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18641,7 +18641,7 @@
       </c>
       <c r="B368" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="369" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18650,7 +18650,7 @@
       </c>
       <c r="B369" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>27</v>
+        <v>76</v>
       </c>
     </row>
     <row r="370" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18659,7 +18659,7 @@
       </c>
       <c r="B370" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="371" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18668,7 +18668,7 @@
       </c>
       <c r="B371" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="372" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18677,7 +18677,7 @@
       </c>
       <c r="B372" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="373" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18686,7 +18686,7 @@
       </c>
       <c r="B373" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="374" spans="1:2" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18695,7 +18695,7 @@
       </c>
       <c r="B374" s="14">
         <f t="shared" ca="1" si="5"/>
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -18720,7 +18720,7 @@
       <selection activeCell="C42" sqref="C42"/>
       <selection pane="topRight" activeCell="C42" sqref="C42"/>
       <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
-      <selection pane="bottomRight" activeCell="L725" sqref="L725"/>
+      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>